<commit_message>
Nye protokoller, metadatasett osv.
</commit_message>
<xml_diff>
--- a/Datagrunnlag/Rådata/Bestanddeler.xlsx
+++ b/Datagrunnlag/Rådata/Bestanddeler.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="103">
   <si>
     <t>Vann</t>
   </si>
@@ -202,13 +202,136 @@
   </si>
   <si>
     <t>Manglende verdi, ukjent innhold.</t>
+  </si>
+  <si>
+    <t>URI</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#betakaroten</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#spiseligDel</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#vann</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#kilojoule</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#kilokalorier</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#fett</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#mettet</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#trans</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#enumettet</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#flerumettet</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#kolesterol</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#karbohydrat</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#stivelse</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#monoDisakk</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#sukkerTilsatt</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#kostfiber</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#protein</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#salt</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#alkohol</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#retinol</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#vitaminA</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#vitaminE</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#vitaminD</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#tiamin</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#riboflavin</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#niacin</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#vitaminB6</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#folat</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#vitaminB12</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#vitaminC</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#kalsium</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#jern</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#natrium</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#kalium</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#magnesium</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#sink</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#selen</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#kobber</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#fosfor</t>
+  </si>
+  <si>
+    <t>http://www.mesan.no/semantisk-web#jod</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +354,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -260,10 +390,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -292,8 +426,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -586,33 +724,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BK41"/>
+  <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.28515625" customWidth="1"/>
+    <col min="1" max="2" width="57.85546875" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="74.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" s="4" customFormat="1" ht="12.75">
+    <row r="1" spans="1:64" s="4" customFormat="1" ht="12.75">
       <c r="A1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="G1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -666,23 +807,26 @@
       <c r="BH1" s="5"/>
       <c r="BI1" s="5"/>
       <c r="BJ1" s="5"/>
-      <c r="BK1" s="3"/>
-    </row>
-    <row r="2" spans="1:63" s="4" customFormat="1" ht="12.75">
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="3"/>
+    </row>
+    <row r="2" spans="1:64" s="4" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="G2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -736,558 +880,719 @@
       <c r="BH2" s="5"/>
       <c r="BI2" s="5"/>
       <c r="BJ2" s="5"/>
-      <c r="BK2" s="3"/>
-    </row>
-    <row r="3" spans="1:63" s="2" customFormat="1" ht="12.75">
+      <c r="BK2" s="5"/>
+      <c r="BL2" s="3"/>
+    </row>
+    <row r="3" spans="1:64" s="2" customFormat="1">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:63">
+      <c r="D3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:64">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:63" s="6" customFormat="1">
+    <row r="5" spans="1:64" s="6" customFormat="1">
       <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:63" s="6" customFormat="1">
+    <row r="6" spans="1:64" s="6" customFormat="1">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:63">
+      <c r="D6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64">
       <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:63">
+      <c r="D7" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:63">
+    <row r="9" spans="1:64">
       <c r="A9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:63">
+      <c r="D9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:64">
       <c r="A10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:63">
+      <c r="D10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:64">
       <c r="A11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:63">
+      <c r="D11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:64">
       <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:63">
+      <c r="D12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:64">
       <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:63">
+      <c r="D13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:64">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:63">
+      <c r="D14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:64">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:63">
+      <c r="D15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:64">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="D23" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="D24" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="D25" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="D26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="D27" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="D28" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="D30" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="D31" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="D32" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="D33" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="D34" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="D35" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="D36" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="D37" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="D38" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="D39" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="D40" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B22:B41" r:id="rId1" display="http://www.mesan.no/semantisk-web#"/>
+    <hyperlink ref="B2" r:id="rId2" location="spiseligDel"/>
+    <hyperlink ref="B3" r:id="rId3" location="vann"/>
+    <hyperlink ref="B4" r:id="rId4" location="kilojoule"/>
+    <hyperlink ref="B5" r:id="rId5" location="kilokalorier"/>
+    <hyperlink ref="B6" r:id="rId6" location="fett"/>
+    <hyperlink ref="B7" r:id="rId7" location="mettet"/>
+    <hyperlink ref="B8" r:id="rId8" location="trans"/>
+    <hyperlink ref="B9" r:id="rId9" location="enumettet"/>
+    <hyperlink ref="B10" r:id="rId10" location="flerumettet"/>
+    <hyperlink ref="B11" r:id="rId11" location="kolesterol"/>
+    <hyperlink ref="B12" r:id="rId12" location="karbohydrat"/>
+    <hyperlink ref="B13" r:id="rId13" location="stivelse"/>
+    <hyperlink ref="B14" r:id="rId14" location="monoDisakk"/>
+    <hyperlink ref="B15" r:id="rId15" location="sukkerTilsatt"/>
+    <hyperlink ref="B16" r:id="rId16" location="kostfiber"/>
+    <hyperlink ref="B17" r:id="rId17" location="protein"/>
+    <hyperlink ref="B18" r:id="rId18" location="salt"/>
+    <hyperlink ref="B19" r:id="rId19" location="alkohol"/>
+    <hyperlink ref="B20" r:id="rId20" location="retinol"/>
+    <hyperlink ref="B21" r:id="rId21" location="betakaroten"/>
+    <hyperlink ref="B22" r:id="rId22" location="vitaminA"/>
+    <hyperlink ref="B23" r:id="rId23" location="vitaminD"/>
+    <hyperlink ref="B24" r:id="rId24" location="vitaminE"/>
+    <hyperlink ref="B25" r:id="rId25" location="tiamin"/>
+    <hyperlink ref="B26" r:id="rId26" location="riboflavin"/>
+    <hyperlink ref="B27" r:id="rId27" location="niacin"/>
+    <hyperlink ref="B28" r:id="rId28" location="vitaminB6"/>
+    <hyperlink ref="B29" r:id="rId29" location="folat"/>
+    <hyperlink ref="B30" r:id="rId30" location="vitaminB12"/>
+    <hyperlink ref="B31" r:id="rId31" location="vitaminC"/>
+    <hyperlink ref="B32" r:id="rId32" location="kalsium"/>
+    <hyperlink ref="B33" r:id="rId33" location="jern"/>
+    <hyperlink ref="B34" r:id="rId34" location="natrium"/>
+    <hyperlink ref="B35" r:id="rId35" location="kalium"/>
+    <hyperlink ref="B36" r:id="rId36" location="magnesium"/>
+    <hyperlink ref="B37" r:id="rId37" location="sink"/>
+    <hyperlink ref="B38" r:id="rId38" location="selen"/>
+    <hyperlink ref="B39" r:id="rId39" location="kobber"/>
+    <hyperlink ref="B40" r:id="rId40" location="fosfor"/>
+    <hyperlink ref="B41" r:id="rId41" location="jod"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
 

</xml_diff>